<commit_message>
Fixed Them BiTich Hon Phoi
</commit_message>
<xml_diff>
--- a/public/excels/ImportTuSi.xlsx
+++ b/public/excels/ImportTuSi.xlsx
@@ -19,6 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="ChucVu">'Các lựa chọn'!$A$2:$A$4</definedName>
+    <definedName name="Gioi_Tinh">'Các lựa chọn'!$D$2:$D$3</definedName>
+    <definedName name="GioiTinh">'Các lựa chọn'!#REF!</definedName>
     <definedName name="TenChucVu">'Các lựa chọn'!$A:$A</definedName>
     <definedName name="TenDong">'Các lựa chọn'!$B:$B</definedName>
     <definedName name="TenThanh">'Các lựa chọn'!$C:$C</definedName>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="116">
   <si>
     <t>Tên chức vụ</t>
   </si>
@@ -372,6 +374,15 @@
   </si>
   <si>
     <t>Hải Dương</t>
+  </si>
+  <si>
+    <t>Giới tính</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Nữ</t>
   </si>
 </sst>
 </file>
@@ -715,34 +726,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.125" customWidth="1"/>
-    <col min="2" max="2" width="9.75" customWidth="1"/>
-    <col min="3" max="3" width="16.25" customWidth="1"/>
-    <col min="4" max="4" width="15.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="16.125" customWidth="1"/>
-    <col min="10" max="10" width="14.25" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="15.125" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="13.25" customWidth="1"/>
-    <col min="15" max="15" width="10.25" customWidth="1"/>
-    <col min="16" max="16" width="18.625" customWidth="1"/>
-    <col min="17" max="17" width="17.75" customWidth="1"/>
+    <col min="2" max="3" width="9.75" customWidth="1"/>
+    <col min="4" max="4" width="16.25" customWidth="1"/>
+    <col min="5" max="5" width="15.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.75" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="16.125" customWidth="1"/>
+    <col min="11" max="11" width="14.25" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="15.125" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="13.25" customWidth="1"/>
+    <col min="16" max="16" width="10.25" customWidth="1"/>
+    <col min="17" max="17" width="18.625" customWidth="1"/>
+    <col min="18" max="18" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -750,335 +761,359 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>25892</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>40198</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>53</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>44</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>112</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>44550</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>25588</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>40198</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>21</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>44</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>112</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="1">
         <v>44550</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>25893</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>40502</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>1</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>21</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>44</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>112</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" t="s">
+      <c r="Q4" s="1"/>
+      <c r="R4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>27429</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>40198</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>53</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>21</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>41</v>
       </c>
-      <c r="P5" s="1">
+      <c r="Q5" s="1">
         <v>44550</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>25569</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>40198</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>1</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>21</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>0</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>41</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>42</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="1">
+      <c r="Q6" s="1">
         <v>44216</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>25708</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>40198</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>1</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>21</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>41</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>42</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>43</v>
       </c>
-      <c r="P7" s="1">
+      <c r="Q7" s="1">
         <v>44206</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576">
       <formula1>ChucVu</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
       <formula1>TenDong</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
       <formula1>TenThanh</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+      <formula1>Gioi_Tinh</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -1277,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1288,12 +1323,11 @@
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="13.125" customWidth="1"/>
     <col min="3" max="3" width="25.125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.875" customWidth="1"/>
-    <col min="5" max="5" width="11.125" customWidth="1"/>
-    <col min="6" max="7" width="11.375" customWidth="1"/>
+    <col min="4" max="4" width="11.125" customWidth="1"/>
+    <col min="5" max="6" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1303,8 +1337,11 @@
       <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1314,8 +1351,11 @@
       <c r="C2" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1325,8 +1365,11 @@
       <c r="C3" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1337,7 +1380,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>59</v>
       </c>
@@ -1345,57 +1388,57 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
         <v>74</v>
       </c>

</xml_diff>